<commit_message>
Auto-committed on 2022/10/18 週二 17:45:40.81
</commit_message>
<xml_diff>
--- a/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
+++ b/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
@@ -1092,8 +1092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/10/31 週一 10:02:02.26
</commit_message>
<xml_diff>
--- a/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
+++ b/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
@@ -15,7 +15,7 @@
     <sheet name="正常件" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">正常件!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">正常件!$A$1:$Q$1</definedName>
     <definedName name="_xlnm.Database" localSheetId="0">正常件!$A$1:$M$1</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve"> 目前生效日  </t>
   </si>
@@ -111,10 +111,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>利率種類</t>
+  </si>
+  <si>
+    <t>地區別上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>地區別下限</t>
-  </si>
-  <si>
-    <t>地區別上限</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1090,11 +1094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1106,19 +1110,20 @@
     <col min="9" max="10" width="11.88671875" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="10.109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="25.44140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" style="1" customWidth="1"/>
-    <col min="16" max="18" width="12.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="1"/>
-    <col min="23" max="23" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="1"/>
+    <col min="13" max="13" width="10.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" style="1" customWidth="1"/>
+    <col min="17" max="19" width="12.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="1"/>
+    <col min="24" max="24" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1159,36 +1164,39 @@
         <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="R1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-committed on 2022/12/09 週五 17:15:29.38
</commit_message>
<xml_diff>
--- a/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
+++ b/Program/Other/L4320_LNW171E底稿(10909調息檔)定期機動-地區別調整.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Database" localSheetId="0">正常件!$A$1:$M$1</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -1098,7 +1098,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>